<commit_message>
Edited inventory file for ed11-t05
</commit_message>
<xml_diff>
--- a/page/eb11/t05/eb11-t05.xlsx
+++ b/page/eb11/t05/eb11-t05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LIB-DSC-FS\Peter Logan\eb-corpus\production\eb11\t05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\knowledge-project\kp2\kp2\page\eb11\t05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FC3A7E-5650-40C2-84F7-0FA2956AB2CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB78D6E-1856-4973-9A7F-01A90D69C21F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="5325" windowWidth="23190" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="s05" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="202">
   <si>
     <t>image-fn.jp2</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t>table</t>
+  </si>
+  <si>
+    <t>mh &amp; tg</t>
+  </si>
+  <si>
+    <t>Complex table structure requires additional attention</t>
   </si>
 </sst>
 </file>
@@ -1009,8 +1015,8 @@
   <dimension ref="A1:L263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,6 +1081,9 @@
         <v>185</v>
       </c>
       <c r="E2" s="5"/>
+      <c r="F2" t="s">
+        <v>200</v>
+      </c>
       <c r="H2" s="13"/>
       <c r="I2" s="16"/>
       <c r="J2" s="5"/>
@@ -2456,7 +2465,9 @@
       <c r="I77" s="16"/>
       <c r="J77" s="5"/>
       <c r="K77" s="18"/>
-      <c r="L77" s="3"/>
+      <c r="L77" s="3" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>

</xml_diff>